<commit_message>
Y axis Rails M3X3030 T-Nut description fixed
</commit_message>
<xml_diff>
--- a/bom/BOM_XY_HD12_SPAWD.xlsx
+++ b/bom/BOM_XY_HD12_SPAWD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="11_2A418477320FE7D5580CDC5AACB522523275C160" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73CB15BE-907B-4B74-930B-F3B346258821}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="11_2A418477320FE7D5580CDC5AACB522523275C160" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8063211D-204E-43B1-9F23-79022240A0CB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="10320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>M3X3030_TSlot_Nut</t>
-  </si>
-  <si>
-    <t>Nut, TSlot - M5X3030</t>
   </si>
   <si>
     <t>M3X10_CapScrew_92290A115</t>
@@ -596,6 +593,9 @@
   </si>
   <si>
     <t>https://s.click.aliexpress.com/e/_DFuQmVt</t>
+  </si>
+  <si>
+    <t>Nut, TSlot - M3X3030</t>
   </si>
 </sst>
 </file>
@@ -3574,8 +3574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3603,26 +3603,26 @@
         <v>LINK TO CAD</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
       <c r="K1" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" ht="23.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>0</v>
@@ -3631,19 +3631,19 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>3</v>
@@ -3654,10 +3654,10 @@
     </row>
     <row r="3" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="22">
         <v>1.1000000000000001</v>
@@ -3667,19 +3667,19 @@
         <v>5</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>7</v>
@@ -3690,10 +3690,10 @@
     </row>
     <row r="4" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="22">
         <v>1.2</v>
@@ -3703,29 +3703,29 @@
         <v>70</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>63</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="22">
         <v>1.2</v>
@@ -3735,29 +3735,29 @@
         <v>73</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>63</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K5" s="14"/>
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="22">
         <v>1.2</v>
@@ -3776,7 +3776,7 @@
         <v>16</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" s="27"/>
       <c r="K6" s="14"/>
@@ -3784,20 +3784,20 @@
     </row>
     <row r="7" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="22">
         <v>1.2</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="24" t="s">
         <v>125</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>126</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>6</v>
@@ -3806,7 +3806,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="14"/>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="8" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C8" s="22">
         <v>2</v>
@@ -3836,7 +3836,7 @@
         <v>16</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J8" s="27"/>
       <c r="K8" s="14" t="s">
@@ -3848,10 +3848,10 @@
     </row>
     <row r="9" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C9" s="22">
         <v>3</v>
@@ -3870,7 +3870,7 @@
         <v>30</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J9" s="27"/>
       <c r="K9" s="14" t="s">
@@ -3882,10 +3882,10 @@
     </row>
     <row r="10" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C10" s="22">
         <v>4</v>
@@ -3902,7 +3902,7 @@
         <v>12</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="14" t="s">
@@ -3914,10 +3914,10 @@
     </row>
     <row r="11" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C11" s="22">
         <v>5</v>
@@ -3934,7 +3934,7 @@
         <v>12</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J11" s="27"/>
       <c r="K11" s="14" t="s">
@@ -3946,10 +3946,10 @@
     </row>
     <row r="12" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C12" s="22">
         <v>6</v>
@@ -3968,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J12" s="27"/>
       <c r="K12" s="14" t="s">
@@ -3980,10 +3980,10 @@
     </row>
     <row r="13" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C13" s="22">
         <v>7</v>
@@ -3993,7 +3993,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="22" t="s">
         <v>6</v>
@@ -4002,7 +4002,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J13" s="27"/>
       <c r="K13" s="14" t="s">
@@ -4014,10 +4014,10 @@
     </row>
     <row r="14" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C14" s="22">
         <v>8</v>
@@ -4027,7 +4027,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>6</v>
@@ -4036,7 +4036,7 @@
         <v>4</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J14" s="27"/>
       <c r="K14" s="14" t="s">
@@ -4048,10 +4048,10 @@
     </row>
     <row r="15" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C15" s="22">
         <v>9</v>
@@ -4066,7 +4066,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J15" s="27"/>
       <c r="K15" s="14"/>
@@ -4074,10 +4074,10 @@
     </row>
     <row r="16" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C16" s="22">
         <v>10</v>
@@ -4096,7 +4096,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J16" s="27"/>
       <c r="K16" s="14"/>
@@ -4104,10 +4104,10 @@
     </row>
     <row r="17" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C17" s="22">
         <v>11</v>
@@ -4126,7 +4126,7 @@
         <v>4</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J17" s="27"/>
       <c r="K17" s="14"/>
@@ -4134,10 +4134,10 @@
     </row>
     <row r="18" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C18" s="22">
         <v>12</v>
@@ -4147,7 +4147,7 @@
         <v>12</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>6</v>
@@ -4156,10 +4156,10 @@
         <v>2</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>13</v>
@@ -4170,10 +4170,10 @@
     </row>
     <row r="19" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C19" s="22">
         <v>15</v>
@@ -4183,7 +4183,7 @@
         <v>57</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>6</v>
@@ -4192,10 +4192,10 @@
         <v>6</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>13</v>
@@ -4206,10 +4206,10 @@
     </row>
     <row r="20" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C20" s="22">
         <v>13</v>
@@ -4219,7 +4219,7 @@
         <v>25</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>6</v>
@@ -4228,10 +4228,10 @@
         <v>4</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>13</v>
@@ -4242,10 +4242,10 @@
     </row>
     <row r="21" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C21" s="22">
         <v>14</v>
@@ -4264,10 +4264,10 @@
         <v>2</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>13</v>
@@ -4278,10 +4278,10 @@
     </row>
     <row r="22" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C22" s="22">
         <v>16</v>
@@ -4300,7 +4300,7 @@
         <v>8</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J22" s="27"/>
       <c r="K22" s="14" t="s">
@@ -4312,10 +4312,10 @@
     </row>
     <row r="23" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C23" s="22">
         <v>17</v>
@@ -4334,7 +4334,7 @@
         <v>4</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J23" s="27"/>
       <c r="K23" s="14" t="s">
@@ -4346,10 +4346,10 @@
     </row>
     <row r="24" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C24" s="22">
         <v>18</v>
@@ -4368,7 +4368,7 @@
         <v>26</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J24" s="27"/>
       <c r="K24" s="14" t="s">
@@ -4380,10 +4380,10 @@
     </row>
     <row r="25" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C25" s="22">
         <v>19</v>
@@ -4402,10 +4402,10 @@
         <v>26</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K25" s="14" t="s">
         <v>13</v>
@@ -4416,10 +4416,10 @@
     </row>
     <row r="26" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C26" s="22">
         <v>20</v>
@@ -4438,22 +4438,22 @@
         <v>1</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J26" s="27"/>
       <c r="K26" s="14" t="s">
         <v>13</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C27" s="22">
         <v>21</v>
@@ -4470,7 +4470,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J27" s="27"/>
       <c r="K27" s="14"/>
@@ -4478,10 +4478,10 @@
     </row>
     <row r="28" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C28" s="22">
         <v>22</v>
@@ -4500,7 +4500,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J28" s="27"/>
       <c r="K28" s="14"/>
@@ -4508,10 +4508,10 @@
     </row>
     <row r="29" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C29" s="22">
         <v>23</v>
@@ -4521,19 +4521,19 @@
         <v>66</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G29" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H29" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J29" s="26" t="s">
         <v>115</v>
-      </c>
-      <c r="I29" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="J29" s="26" t="s">
-        <v>116</v>
       </c>
       <c r="K29" s="14" t="s">
         <v>67</v>
@@ -4544,10 +4544,10 @@
     </row>
     <row r="30" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C30" s="22">
         <v>24</v>
@@ -4557,19 +4557,19 @@
         <v>69</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G30" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H30" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J30" s="26" t="s">
         <v>115</v>
-      </c>
-      <c r="I30" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="J30" s="26" t="s">
-        <v>116</v>
       </c>
       <c r="K30" s="14" t="s">
         <v>67</v>
@@ -4580,10 +4580,10 @@
     </row>
     <row r="31" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C31" s="22">
         <v>25</v>
@@ -4602,20 +4602,20 @@
         <v>2</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K31" s="14"/>
       <c r="L31" s="18"/>
     </row>
     <row r="32" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C32" s="22">
         <v>26</v>
@@ -4634,20 +4634,20 @@
         <v>2</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K32" s="14"/>
       <c r="L32" s="18"/>
     </row>
     <row r="33" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C33" s="22">
         <v>27</v>
@@ -4657,65 +4657,65 @@
         <v>77</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="G33" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I33" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J33" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K33" s="14" t="s">
         <v>13</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C34" s="22">
         <v>28</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="24" t="s">
         <v>79</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="G34" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H34" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J34" s="28" t="s">
         <v>127</v>
-      </c>
-      <c r="I34" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="J34" s="28" t="s">
-        <v>128</v>
       </c>
       <c r="K34" s="15"/>
       <c r="L34" s="19"/>
     </row>
     <row r="35" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C35" s="22">
         <v>29</v>
@@ -4725,7 +4725,7 @@
         <v>49</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G35" s="22" t="s">
         <v>63</v>
@@ -4734,7 +4734,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J35" s="27"/>
       <c r="K35" s="14" t="s">
@@ -4744,10 +4744,10 @@
     </row>
     <row r="36" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C36" s="22">
         <v>30</v>
@@ -4757,7 +4757,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G36" s="22" t="s">
         <v>63</v>
@@ -4766,7 +4766,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J36" s="27"/>
       <c r="K36" s="14" t="s">
@@ -4776,10 +4776,10 @@
     </row>
     <row r="37" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="C37" s="22">
         <v>31</v>
@@ -4789,7 +4789,7 @@
         <v>51</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G37" s="22" t="s">
         <v>63</v>
@@ -4798,7 +4798,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J37" s="27"/>
       <c r="K37" s="14" t="s">
@@ -4808,10 +4808,10 @@
     </row>
     <row r="38" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="22">
         <v>32</v>
@@ -4821,7 +4821,7 @@
         <v>58</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G38" s="22" t="s">
         <v>63</v>
@@ -4830,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J38" s="27"/>
       <c r="K38" s="14" t="s">
@@ -4840,10 +4840,10 @@
     </row>
     <row r="39" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="22">
         <v>33</v>
@@ -4853,7 +4853,7 @@
         <v>59</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G39" s="22" t="s">
         <v>63</v>
@@ -4862,7 +4862,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J39" s="27"/>
       <c r="K39" s="14" t="s">
@@ -4872,10 +4872,10 @@
     </row>
     <row r="40" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="22">
         <v>34</v>
@@ -4885,7 +4885,7 @@
         <v>60</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G40" s="22" t="s">
         <v>63</v>
@@ -4894,7 +4894,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J40" s="27"/>
       <c r="K40" s="14" t="s">
@@ -4904,10 +4904,10 @@
     </row>
     <row r="41" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="22">
         <v>35</v>
@@ -4917,7 +4917,7 @@
         <v>61</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G41" s="22" t="s">
         <v>63</v>
@@ -4926,7 +4926,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J41" s="27"/>
       <c r="K41" s="14" t="s">
@@ -4936,20 +4936,20 @@
     </row>
     <row r="42" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="22">
         <v>36</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F42" s="24" t="s">
         <v>108</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>109</v>
       </c>
       <c r="G42" s="22" t="s">
         <v>63</v>
@@ -4958,7 +4958,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J42" s="27"/>
       <c r="K42" s="14" t="s">
@@ -4968,10 +4968,10 @@
     </row>
     <row r="43" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C43" s="22">
         <v>37</v>
@@ -4981,7 +4981,7 @@
         <v>62</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G43" s="22" t="s">
         <v>63</v>
@@ -4990,7 +4990,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J43" s="27"/>
       <c r="K43" s="14" t="s">
@@ -5000,10 +5000,10 @@
     </row>
     <row r="44" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C44" s="22">
         <v>38</v>
@@ -5013,7 +5013,7 @@
         <v>65</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G44" s="22" t="s">
         <v>63</v>
@@ -5022,7 +5022,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J44" s="27"/>
       <c r="K44" s="14" t="s">

</xml_diff>

<commit_message>
Added 5X1 washer under each Motor Pulley
</commit_message>
<xml_diff>
--- a/bom/BOM_XY_HD12_SPAWD.xlsx
+++ b/bom/BOM_XY_HD12_SPAWD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="11_2A418477320FE7D5580CDC5AACB522523275C160" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8063211D-204E-43B1-9F23-79022240A0CB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E3F117-B9FC-46B4-856B-A32668A9EE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="10320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="133">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>Nut, TSlot - M3X3030</t>
+  </si>
+  <si>
+    <t>12 for motor covers and 4 for uner motor pulleys to act as height reference surface.</t>
   </si>
 </sst>
 </file>
@@ -3574,8 +3577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3931,12 +3934,14 @@
         <v>6</v>
       </c>
       <c r="H11" s="22">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I11" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="J11" s="27"/>
+      <c r="J11" s="27" t="s">
+        <v>132</v>
+      </c>
       <c r="K11" s="14" t="s">
         <v>13</v>
       </c>
@@ -5059,7 +5064,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId20"/>
   <webPublishItems count="1">
-    <webPublishItem id="30499" divId="BOM_XY_HD12_SPAWD_30499" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_XY_HD12_SPAWD.htm" autoRepublish="1"/>
+    <webPublishItem id="30499" divId="BOM_XY_HD12_SPAWD_30499" sourceType="sheet" destinationFile="C:\Users\olivi\HevORT\bom\BOM_XY_HD12_SPAWD.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId21"/>

</xml_diff>